<commit_message>
update DDL_UnitTestCase_SlideRepository_v1.0.xlsx add DDL_UnitTestCase_CategoryRepository_v1.0.xlsx
</commit_message>
<xml_diff>
--- a/WIP/Users/ManhLN/Report 4/UT/DDL_UnitTestCase_SlideRepository_v1.0.xlsx
+++ b/WIP/Users/ManhLN/Report 4/UT/DDL_UnitTestCase_SlideRepository_v1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="886" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="886" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Guidleline" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="9">ChangeSlideStatus!$A$1:$Q$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">CreateSlide!$A$1:$Q$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">DeleteSlide!$A$1:$Q$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">EditSlide!$A$1:$Q$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">EditSlide!$A$1:$Q$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">FunctionList!$A$1:$H$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">GetSlides!$A$1:$Q$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">GetSlidesForAdmin!$A$1:$Q$35</definedName>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="159">
   <si>
     <t>Project Name</t>
   </si>
@@ -757,6 +757,15 @@
   </si>
   <si>
     <t>UTCID06</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>"new title"</t>
   </si>
 </sst>
 </file>
@@ -2729,6 +2738,9 @@
     <xf numFmtId="1" fontId="12" fillId="24" borderId="14" xfId="67" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="28" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2790,6 +2802,72 @@
     <xf numFmtId="14" fontId="39" fillId="24" borderId="10" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="51" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="52" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="53" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="48" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="49" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="54" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="43" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="55" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="56" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="28" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="29" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="30" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="57" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="61" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="62" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="50" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="24" borderId="63" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2861,75 +2939,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="24" borderId="27" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="51" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="52" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="53" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="48" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="49" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="54" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="43" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="55" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="56" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="28" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="29" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="30" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="78" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="57" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="61" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="62" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="50" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="30" borderId="28" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="90">
@@ -5364,7 +5373,7 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -5384,136 +5393,136 @@
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="185" t="s">
+      <c r="B2" s="207"/>
+      <c r="C2" s="208" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="186"/>
-      <c r="E2" s="201" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="224" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="191" t="str">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="214" t="str">
         <f>C2</f>
         <v>ChangeSlideStatus</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="193"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
+      <c r="O2" s="215"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="216"/>
       <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="197" t="str">
+      <c r="B3" s="213"/>
+      <c r="C3" s="220" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="D3" s="198"/>
-      <c r="E3" s="204" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="227" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="194" t="str">
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
+      <c r="I3" s="217" t="str">
         <f>C3</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="196"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218"/>
+      <c r="R3" s="219"/>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="210"/>
-      <c r="K4" s="210"/>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
-      <c r="N4" s="210"/>
-      <c r="O4" s="210"/>
-      <c r="P4" s="210"/>
-      <c r="Q4" s="210"/>
-      <c r="R4" s="212"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="189"/>
     </row>
     <row r="5" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="228" t="s">
+      <c r="B5" s="223"/>
+      <c r="C5" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="213" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="214"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="214" t="s">
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="214"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="213" t="s">
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="190" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="214"/>
-      <c r="N5" s="214"/>
-      <c r="O5" s="214"/>
-      <c r="P5" s="214"/>
-      <c r="Q5" s="214"/>
-      <c r="R5" s="215"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="192"/>
       <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="187">
+      <c r="A6" s="210">
         <f>COUNTIF(E22:HM22,"P")</f>
         <v>3</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="227">
+      <c r="B6" s="211"/>
+      <c r="C6" s="204">
         <f>COUNTIF(E22:HO22,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="216">
+      <c r="D6" s="194"/>
+      <c r="E6" s="193">
         <f>SUM(L6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="217"/>
-      <c r="G6" s="217"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="148">
         <f>COUNTIF(E21:HM21,"N")</f>
         <v>2</v>
@@ -5526,16 +5535,16 @@
         <f>COUNTIF(E21:HO21,"B")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="216">
+      <c r="L6" s="193">
         <f>COUNTA(E8:R8)</f>
         <v>3</v>
       </c>
-      <c r="M6" s="217"/>
-      <c r="N6" s="217"/>
-      <c r="O6" s="217"/>
-      <c r="P6" s="217"/>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="218"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="149"/>
     </row>
     <row r="7" spans="1:20" ht="11.25" thickBot="1"/>
@@ -5575,7 +5584,9 @@
       </c>
       <c r="C9" s="117"/>
       <c r="D9" s="118"/>
-      <c r="E9" s="125"/>
+      <c r="E9" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="F9" s="106"/>
       <c r="G9" s="106"/>
       <c r="H9" s="125"/>
@@ -5599,7 +5610,9 @@
       <c r="D10" s="118"/>
       <c r="E10" s="125"/>
       <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
+      <c r="G10" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="H10" s="125"/>
       <c r="I10" s="125"/>
       <c r="J10" s="125"/>
@@ -5620,7 +5633,9 @@
       <c r="C11" s="117"/>
       <c r="D11" s="118"/>
       <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
+      <c r="F11" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="G11" s="125"/>
       <c r="H11" s="125"/>
       <c r="I11" s="125"/>
@@ -5864,11 +5879,11 @@
       <c r="A21" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="219" t="s">
+      <c r="B21" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="220"/>
-      <c r="D21" s="221"/>
+      <c r="C21" s="197"/>
+      <c r="D21" s="198"/>
       <c r="E21" s="158" t="s">
         <v>37</v>
       </c>
@@ -5892,11 +5907,11 @@
     </row>
     <row r="22" spans="1:18" ht="13.5" customHeight="1">
       <c r="A22" s="113"/>
-      <c r="B22" s="222" t="s">
+      <c r="B22" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="223"/>
-      <c r="D22" s="224"/>
+      <c r="C22" s="200"/>
+      <c r="D22" s="201"/>
       <c r="E22" s="106" t="s">
         <v>41</v>
       </c>
@@ -5920,11 +5935,11 @@
     </row>
     <row r="23" spans="1:18" ht="64.5" customHeight="1">
       <c r="A23" s="113"/>
-      <c r="B23" s="207" t="s">
+      <c r="B23" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="208"/>
-      <c r="D23" s="209"/>
+      <c r="C23" s="185"/>
+      <c r="D23" s="186"/>
       <c r="E23" s="86">
         <v>42335</v>
       </c>
@@ -5956,20 +5971,6 @@
     <row r="56" ht="10.5"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="L6:R6"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:R5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -5978,6 +5979,20 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:R3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11 I9:I10 E12:R20 E9:G11">
@@ -6002,8 +6017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -6023,136 +6038,136 @@
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="185" t="s">
+      <c r="B2" s="207"/>
+      <c r="C2" s="208" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="186"/>
-      <c r="E2" s="201" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="224" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="191" t="str">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="214" t="str">
         <f>C2</f>
         <v>ChangeOrder</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="193"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
+      <c r="O2" s="215"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="216"/>
       <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="197" t="str">
+      <c r="B3" s="213"/>
+      <c r="C3" s="220" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="D3" s="198"/>
-      <c r="E3" s="204" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="227" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="194" t="str">
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
+      <c r="I3" s="217" t="str">
         <f>C3</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="196"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218"/>
+      <c r="R3" s="219"/>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="210"/>
-      <c r="K4" s="210"/>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
-      <c r="N4" s="210"/>
-      <c r="O4" s="210"/>
-      <c r="P4" s="210"/>
-      <c r="Q4" s="210"/>
-      <c r="R4" s="212"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="189"/>
     </row>
     <row r="5" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="228" t="s">
+      <c r="B5" s="223"/>
+      <c r="C5" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="213" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="214"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="214" t="s">
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="214"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="213" t="s">
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="190" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="214"/>
-      <c r="N5" s="214"/>
-      <c r="O5" s="214"/>
-      <c r="P5" s="214"/>
-      <c r="Q5" s="214"/>
-      <c r="R5" s="215"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="192"/>
       <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="187">
+      <c r="A6" s="210">
         <f>COUNTIF(E35:HM35,"P")</f>
         <v>6</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="227">
+      <c r="B6" s="211"/>
+      <c r="C6" s="204">
         <f>COUNTIF(E35:HO35,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="216">
+      <c r="D6" s="194"/>
+      <c r="E6" s="193">
         <f>SUM(L6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="217"/>
-      <c r="G6" s="217"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="148">
         <f>COUNTIF(E34:HM34,"N")</f>
         <v>3</v>
@@ -6165,16 +6180,16 @@
         <f>COUNTIF(E34:HO34,"B")</f>
         <v>2</v>
       </c>
-      <c r="L6" s="216">
+      <c r="L6" s="193">
         <f>COUNTA(E8:R8)</f>
         <v>6</v>
       </c>
-      <c r="M6" s="217"/>
-      <c r="N6" s="217"/>
-      <c r="O6" s="217"/>
-      <c r="P6" s="217"/>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="218"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="149"/>
     </row>
     <row r="7" spans="1:20" ht="11.25" thickBot="1"/>
@@ -6220,10 +6235,16 @@
       </c>
       <c r="C9" s="117"/>
       <c r="D9" s="118"/>
-      <c r="E9" s="125"/>
+      <c r="E9" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="125"/>
+      <c r="G9" s="106" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="106" t="s">
+        <v>71</v>
+      </c>
       <c r="I9" s="125"/>
       <c r="J9" s="125"/>
       <c r="K9" s="124"/>
@@ -6244,10 +6265,14 @@
       <c r="D10" s="118"/>
       <c r="E10" s="125"/>
       <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
+      <c r="G10" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="H10" s="125"/>
       <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
+      <c r="J10" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="K10" s="124"/>
       <c r="L10" s="124"/>
       <c r="M10" s="150"/>
@@ -6269,7 +6294,9 @@
       <c r="G11" s="125"/>
       <c r="H11" s="125"/>
       <c r="I11" s="125"/>
-      <c r="J11" s="125"/>
+      <c r="J11" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="K11" s="124"/>
       <c r="L11" s="124"/>
       <c r="M11" s="150"/>
@@ -6290,7 +6317,9 @@
       <c r="F12" s="125"/>
       <c r="G12" s="125"/>
       <c r="H12" s="125"/>
-      <c r="I12" s="125"/>
+      <c r="I12" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="J12" s="125"/>
       <c r="K12" s="124"/>
       <c r="L12" s="124"/>
@@ -6309,7 +6338,9 @@
       <c r="C13" s="117"/>
       <c r="D13" s="118"/>
       <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
+      <c r="F13" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="G13" s="125"/>
       <c r="H13" s="125"/>
       <c r="I13" s="125"/>
@@ -6720,8 +6751,8 @@
       <c r="J29" s="152"/>
       <c r="K29" s="152"/>
       <c r="L29" s="152"/>
-      <c r="M29" s="229"/>
-      <c r="N29" s="229"/>
+      <c r="M29" s="162"/>
+      <c r="N29" s="162"/>
       <c r="O29" s="124"/>
       <c r="P29" s="124"/>
       <c r="Q29" s="124"/>
@@ -6746,8 +6777,8 @@
       </c>
       <c r="K30" s="152"/>
       <c r="L30" s="152"/>
-      <c r="M30" s="229"/>
-      <c r="N30" s="229"/>
+      <c r="M30" s="162"/>
+      <c r="N30" s="162"/>
       <c r="O30" s="124"/>
       <c r="P30" s="124"/>
       <c r="Q30" s="124"/>
@@ -6772,8 +6803,8 @@
       </c>
       <c r="K31" s="152"/>
       <c r="L31" s="152"/>
-      <c r="M31" s="229"/>
-      <c r="N31" s="229"/>
+      <c r="M31" s="162"/>
+      <c r="N31" s="162"/>
       <c r="O31" s="124"/>
       <c r="P31" s="124"/>
       <c r="Q31" s="124"/>
@@ -6792,8 +6823,8 @@
       <c r="J32" s="152"/>
       <c r="K32" s="152"/>
       <c r="L32" s="152"/>
-      <c r="M32" s="229"/>
-      <c r="N32" s="229"/>
+      <c r="M32" s="162"/>
+      <c r="N32" s="162"/>
       <c r="O32" s="124"/>
       <c r="P32" s="124"/>
       <c r="Q32" s="124"/>
@@ -6823,11 +6854,11 @@
       <c r="A34" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="219" t="s">
+      <c r="B34" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="220"/>
-      <c r="D34" s="221"/>
+      <c r="C34" s="197"/>
+      <c r="D34" s="198"/>
       <c r="E34" s="158" t="s">
         <v>37</v>
       </c>
@@ -6857,11 +6888,11 @@
     </row>
     <row r="35" spans="1:18" ht="13.5" customHeight="1">
       <c r="A35" s="113"/>
-      <c r="B35" s="222" t="s">
+      <c r="B35" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="223"/>
-      <c r="D35" s="224"/>
+      <c r="C35" s="200"/>
+      <c r="D35" s="201"/>
       <c r="E35" s="106" t="s">
         <v>41</v>
       </c>
@@ -6891,11 +6922,11 @@
     </row>
     <row r="36" spans="1:18" ht="64.5" customHeight="1">
       <c r="A36" s="113"/>
-      <c r="B36" s="207" t="s">
+      <c r="B36" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="208"/>
-      <c r="D36" s="209"/>
+      <c r="C36" s="185"/>
+      <c r="D36" s="186"/>
       <c r="E36" s="86">
         <v>42335</v>
       </c>
@@ -6933,20 +6964,6 @@
     <row r="69" ht="10.5"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="L6:R6"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:R5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -6955,6 +6972,20 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:R3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E34:R34">
@@ -6963,7 +6994,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E35:R35">
       <formula1>"P,F, "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13 I9:I12 E14:R33 E9:G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13 I9:I12 E14:R33 E9:G13 H9 J10:J11">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>
@@ -6980,7 +7011,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -6999,13 +7030,13 @@
       <c r="A2" s="129" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="166" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="168"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="130"/>
@@ -7019,11 +7050,11 @@
       <c r="A4" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="163" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
       <c r="E4" s="103" t="s">
         <v>1</v>
       </c>
@@ -7035,11 +7066,11 @@
       <c r="A5" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="162" t="s">
+      <c r="B5" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
       <c r="E5" s="103" t="s">
         <v>3</v>
       </c>
@@ -7048,15 +7079,15 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="164" t="str">
+      <c r="B6" s="165" t="str">
         <f>B5&amp;"_UnitTestCase_SlideRepository_v1.0.xls"</f>
         <v>DDL_UnitTestCase_SlideRepository_v1.0.xls</v>
       </c>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
       <c r="E6" s="103" t="s">
         <v>5</v>
       </c>
@@ -7065,10 +7096,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A7" s="163"/>
-      <c r="B7" s="164"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
+      <c r="A7" s="164"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
       <c r="E7" s="103" t="s">
         <v>6</v>
       </c>
@@ -7317,48 +7348,48 @@
       <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A4" s="169" t="s">
+      <c r="A4" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="169"/>
-      <c r="C4" s="169"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="170" t="str">
+      <c r="B4" s="170"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="171" t="str">
         <f>Cover!B4</f>
         <v>Dandelion</v>
       </c>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="173"/>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A5" s="169" t="s">
+      <c r="A5" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="169"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="170" t="str">
+      <c r="B5" s="170"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="171" t="str">
         <f>Cover!B5</f>
         <v>DDL</v>
       </c>
-      <c r="F5" s="171"/>
-      <c r="G5" s="171"/>
-      <c r="H5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="173"/>
     </row>
     <row r="6" spans="1:8" s="26" customFormat="1" ht="80.25" customHeight="1">
-      <c r="A6" s="168" t="s">
+      <c r="A6" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="168"/>
-      <c r="C6" s="168"/>
-      <c r="D6" s="168"/>
-      <c r="E6" s="173" t="s">
+      <c r="B6" s="169"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="174" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="174"/>
-      <c r="G6" s="174"/>
-      <c r="H6" s="175"/>
+      <c r="F6" s="175"/>
+      <c r="G6" s="175"/>
+      <c r="H6" s="176"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="27"/>
@@ -7655,17 +7686,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="25.5" customHeight="1">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="178" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
-      <c r="H2" s="177"/>
-      <c r="I2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
       <c r="A3" s="54"/>
@@ -7682,80 +7713,80 @@
       <c r="A4" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="178" t="str">
+      <c r="B4" s="179" t="str">
         <f>Cover!B4</f>
         <v>Dandelion</v>
       </c>
-      <c r="C4" s="178"/>
-      <c r="D4" s="179" t="s">
+      <c r="C4" s="179"/>
+      <c r="D4" s="180" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="179"/>
-      <c r="F4" s="170" t="str">
+      <c r="E4" s="180"/>
+      <c r="F4" s="171" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="172"/>
+      <c r="I4" s="173"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" customHeight="1">
       <c r="A5" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="178" t="str">
+      <c r="B5" s="179" t="str">
         <f>Cover!B5</f>
         <v>DDL</v>
       </c>
-      <c r="C5" s="178"/>
-      <c r="D5" s="179" t="s">
+      <c r="C5" s="179"/>
+      <c r="D5" s="180" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="179"/>
-      <c r="F5" s="170" t="str">
+      <c r="E5" s="180"/>
+      <c r="F5" s="171" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="172"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="172"/>
+      <c r="I5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" customHeight="1">
       <c r="A6" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="178" t="str">
+      <c r="B6" s="179" t="str">
         <f>B5&amp;"_"&amp;"Test Report"&amp;"_"&amp;"v1.0"</f>
         <v>DDL_Test Report_v1.0</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="179" t="s">
+      <c r="C6" s="179"/>
+      <c r="D6" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="179"/>
-      <c r="F6" s="180">
+      <c r="E6" s="180"/>
+      <c r="F6" s="181">
         <f>Cover!F6</f>
         <v>42335</v>
       </c>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="182"/>
+      <c r="G6" s="182"/>
+      <c r="H6" s="182"/>
+      <c r="I6" s="183"/>
       <c r="J6" s="66"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="176" t="s">
+      <c r="B7" s="177" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="176"/>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
+      <c r="C7" s="177"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
       <c r="A8" s="57"/>
@@ -8277,136 +8308,136 @@
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="185" t="s">
+      <c r="B2" s="207"/>
+      <c r="C2" s="208" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="186"/>
-      <c r="E2" s="201" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="224" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="191" t="str">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="214" t="str">
         <f>C2</f>
         <v>GetSlides</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="193"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
+      <c r="O2" s="215"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="216"/>
       <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="197" t="str">
+      <c r="B3" s="213"/>
+      <c r="C3" s="220" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="D3" s="198"/>
-      <c r="E3" s="204" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="227" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="194" t="str">
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
+      <c r="I3" s="217" t="str">
         <f>C3</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="196"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218"/>
+      <c r="R3" s="219"/>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="210"/>
-      <c r="K4" s="210"/>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
-      <c r="N4" s="210"/>
-      <c r="O4" s="210"/>
-      <c r="P4" s="210"/>
-      <c r="Q4" s="210"/>
-      <c r="R4" s="212"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="189"/>
     </row>
     <row r="5" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="228" t="s">
+      <c r="B5" s="223"/>
+      <c r="C5" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="213" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="214"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="214" t="s">
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="214"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="213" t="s">
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="190" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="214"/>
-      <c r="N5" s="214"/>
-      <c r="O5" s="214"/>
-      <c r="P5" s="214"/>
-      <c r="Q5" s="214"/>
-      <c r="R5" s="215"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="192"/>
       <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="187">
+      <c r="A6" s="210">
         <f>COUNTIF(E20:HM20,"P")</f>
         <v>1</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="227">
+      <c r="B6" s="211"/>
+      <c r="C6" s="204">
         <f>COUNTIF(E20:HO20,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="216">
+      <c r="D6" s="194"/>
+      <c r="E6" s="193">
         <f>SUM(L6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="217"/>
-      <c r="G6" s="217"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="148">
         <f>COUNTIF(E19:HM19,"N")</f>
         <v>1</v>
@@ -8419,16 +8450,16 @@
         <f>COUNTIF(E19:HO19,"B")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="216">
+      <c r="L6" s="193">
         <f>COUNTA(E8:R8)</f>
         <v>1</v>
       </c>
-      <c r="M6" s="217"/>
-      <c r="N6" s="217"/>
-      <c r="O6" s="217"/>
-      <c r="P6" s="217"/>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="218"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="149"/>
     </row>
     <row r="7" spans="1:20" ht="11.25" thickBot="1"/>
@@ -8679,11 +8710,11 @@
       <c r="A19" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="219" t="s">
+      <c r="B19" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="220"/>
-      <c r="D19" s="221"/>
+      <c r="C19" s="197"/>
+      <c r="D19" s="198"/>
       <c r="E19" s="158" t="s">
         <v>37</v>
       </c>
@@ -8703,11 +8734,11 @@
     </row>
     <row r="20" spans="1:18" ht="13.5" customHeight="1">
       <c r="A20" s="113"/>
-      <c r="B20" s="222" t="s">
+      <c r="B20" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="223"/>
-      <c r="D20" s="224"/>
+      <c r="C20" s="200"/>
+      <c r="D20" s="201"/>
       <c r="E20" s="106" t="s">
         <v>41</v>
       </c>
@@ -8727,11 +8758,11 @@
     </row>
     <row r="21" spans="1:18" ht="64.5" customHeight="1">
       <c r="A21" s="113"/>
-      <c r="B21" s="207" t="s">
+      <c r="B21" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="208"/>
-      <c r="D21" s="209"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="186"/>
       <c r="E21" s="86">
         <v>42335</v>
       </c>
@@ -8759,6 +8790,17 @@
     <row r="54" ht="10.5"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="I2:R2"/>
+    <mergeCell ref="I3:R3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="C4:R4"/>
     <mergeCell ref="L5:R5"/>
@@ -8770,17 +8812,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="I2:R2"/>
-    <mergeCell ref="I3:R3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <dataValidations count="3">
@@ -8827,136 +8858,136 @@
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="185" t="s">
+      <c r="B2" s="207"/>
+      <c r="C2" s="208" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="186"/>
-      <c r="E2" s="201" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="224" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="191" t="str">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="214" t="str">
         <f>C2</f>
         <v>GetSlides</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="193"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
+      <c r="O2" s="215"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="216"/>
       <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="197" t="str">
+      <c r="B3" s="213"/>
+      <c r="C3" s="220" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="D3" s="198"/>
-      <c r="E3" s="204" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="227" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="194" t="str">
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
+      <c r="I3" s="217" t="str">
         <f>C3</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="196"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218"/>
+      <c r="R3" s="219"/>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="210"/>
-      <c r="K4" s="210"/>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
-      <c r="N4" s="210"/>
-      <c r="O4" s="210"/>
-      <c r="P4" s="210"/>
-      <c r="Q4" s="210"/>
-      <c r="R4" s="212"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="189"/>
     </row>
     <row r="5" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="228" t="s">
+      <c r="B5" s="223"/>
+      <c r="C5" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="213" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="214"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="214" t="s">
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="214"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="213" t="s">
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="190" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="214"/>
-      <c r="N5" s="214"/>
-      <c r="O5" s="214"/>
-      <c r="P5" s="214"/>
-      <c r="Q5" s="214"/>
-      <c r="R5" s="215"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="192"/>
       <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="187">
+      <c r="A6" s="210">
         <f>COUNTIF(E20:HM20,"P")</f>
         <v>1</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="227">
+      <c r="B6" s="211"/>
+      <c r="C6" s="204">
         <f>COUNTIF(E20:HO20,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="216">
+      <c r="D6" s="194"/>
+      <c r="E6" s="193">
         <f>SUM(L6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="217"/>
-      <c r="G6" s="217"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="148">
         <f>COUNTIF(E19:HM19,"N")</f>
         <v>1</v>
@@ -8969,16 +9000,16 @@
         <f>COUNTIF(E19:HO19,"B")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="216">
+      <c r="L6" s="193">
         <f>COUNTA(E8:R8)</f>
         <v>1</v>
       </c>
-      <c r="M6" s="217"/>
-      <c r="N6" s="217"/>
-      <c r="O6" s="217"/>
-      <c r="P6" s="217"/>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="218"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="149"/>
     </row>
     <row r="7" spans="1:20" ht="11.25" thickBot="1"/>
@@ -9229,11 +9260,11 @@
       <c r="A19" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="219" t="s">
+      <c r="B19" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="220"/>
-      <c r="D19" s="221"/>
+      <c r="C19" s="197"/>
+      <c r="D19" s="198"/>
       <c r="E19" s="158" t="s">
         <v>37</v>
       </c>
@@ -9253,11 +9284,11 @@
     </row>
     <row r="20" spans="1:18" ht="13.5" customHeight="1">
       <c r="A20" s="113"/>
-      <c r="B20" s="222" t="s">
+      <c r="B20" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="223"/>
-      <c r="D20" s="224"/>
+      <c r="C20" s="200"/>
+      <c r="D20" s="201"/>
       <c r="E20" s="106" t="s">
         <v>41</v>
       </c>
@@ -9277,11 +9308,11 @@
     </row>
     <row r="21" spans="1:18" ht="64.5" customHeight="1">
       <c r="A21" s="113"/>
-      <c r="B21" s="207" t="s">
+      <c r="B21" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="208"/>
-      <c r="D21" s="209"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="186"/>
       <c r="E21" s="86">
         <v>42335</v>
       </c>
@@ -9309,20 +9340,6 @@
     <row r="54" ht="10.5"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="L6:R6"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:R5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -9331,6 +9348,20 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:R3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10 I9 E9:G10 E11:R18">
@@ -9355,8 +9386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -9376,136 +9407,136 @@
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="185" t="s">
+      <c r="B2" s="207"/>
+      <c r="C2" s="208" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="186"/>
-      <c r="E2" s="201" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="224" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="191" t="str">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="214" t="str">
         <f>C2</f>
         <v>CreateSlide</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="193"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
+      <c r="O2" s="215"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="216"/>
       <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="197" t="str">
+      <c r="B3" s="213"/>
+      <c r="C3" s="220" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="D3" s="198"/>
-      <c r="E3" s="204" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="227" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="194" t="str">
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
+      <c r="I3" s="217" t="str">
         <f>C3</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="196"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218"/>
+      <c r="R3" s="219"/>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="210"/>
-      <c r="K4" s="210"/>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
-      <c r="N4" s="210"/>
-      <c r="O4" s="210"/>
-      <c r="P4" s="210"/>
-      <c r="Q4" s="210"/>
-      <c r="R4" s="212"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="189"/>
     </row>
     <row r="5" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="228" t="s">
+      <c r="B5" s="223"/>
+      <c r="C5" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="213" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="214"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="214" t="s">
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="214"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="213" t="s">
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="190" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="214"/>
-      <c r="N5" s="214"/>
-      <c r="O5" s="214"/>
-      <c r="P5" s="214"/>
-      <c r="Q5" s="214"/>
-      <c r="R5" s="215"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="192"/>
       <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="187">
+      <c r="A6" s="210">
         <f>COUNTIF(E20:HM20,"P")</f>
         <v>1</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="227">
+      <c r="B6" s="211"/>
+      <c r="C6" s="204">
         <f>COUNTIF(E20:HO20,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="216">
+      <c r="D6" s="194"/>
+      <c r="E6" s="193">
         <f>SUM(L6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="217"/>
-      <c r="G6" s="217"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="148">
         <f>COUNTIF(E19:HM19,"N")</f>
         <v>1</v>
@@ -9518,16 +9549,16 @@
         <f>COUNTIF(E19:HO19,"B")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="216">
+      <c r="L6" s="193">
         <f>COUNTA(E8:R8)</f>
         <v>1</v>
       </c>
-      <c r="M6" s="217"/>
-      <c r="N6" s="217"/>
-      <c r="O6" s="217"/>
-      <c r="P6" s="217"/>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="218"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="149"/>
     </row>
     <row r="7" spans="1:20" ht="11.25" thickBot="1"/>
@@ -9605,7 +9636,7 @@
       </c>
       <c r="C11" s="117"/>
       <c r="D11" s="118"/>
-      <c r="E11" s="124" t="s">
+      <c r="E11" s="125" t="s">
         <v>71</v>
       </c>
       <c r="F11" s="124"/>
@@ -9778,11 +9809,11 @@
       <c r="A19" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="219" t="s">
+      <c r="B19" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="220"/>
-      <c r="D19" s="221"/>
+      <c r="C19" s="197"/>
+      <c r="D19" s="198"/>
       <c r="E19" s="158" t="s">
         <v>37</v>
       </c>
@@ -9802,11 +9833,11 @@
     </row>
     <row r="20" spans="1:18" ht="13.5" customHeight="1">
       <c r="A20" s="113"/>
-      <c r="B20" s="222" t="s">
+      <c r="B20" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="223"/>
-      <c r="D20" s="224"/>
+      <c r="C20" s="200"/>
+      <c r="D20" s="201"/>
       <c r="E20" s="106" t="s">
         <v>41</v>
       </c>
@@ -9826,11 +9857,11 @@
     </row>
     <row r="21" spans="1:18" ht="64.5" customHeight="1">
       <c r="A21" s="113"/>
-      <c r="B21" s="207" t="s">
+      <c r="B21" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="208"/>
-      <c r="D21" s="209"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="186"/>
       <c r="E21" s="86">
         <v>42335</v>
       </c>
@@ -9858,20 +9889,6 @@
     <row r="54" ht="10.5"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="L6:R6"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:R5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -9880,6 +9897,20 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:R3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19:R19">
@@ -9902,10 +9933,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -9925,158 +9956,158 @@
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="185" t="s">
+      <c r="B2" s="207"/>
+      <c r="C2" s="208" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="186"/>
-      <c r="E2" s="201" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="224" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="191" t="str">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="214" t="str">
         <f>C2</f>
         <v>CreateSlide</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="193"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
+      <c r="O2" s="215"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="216"/>
       <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="197" t="str">
+      <c r="B3" s="213"/>
+      <c r="C3" s="220" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="D3" s="198"/>
-      <c r="E3" s="204" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="227" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="194" t="str">
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
+      <c r="I3" s="217" t="str">
         <f>C3</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="196"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218"/>
+      <c r="R3" s="219"/>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="210"/>
-      <c r="K4" s="210"/>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
-      <c r="N4" s="210"/>
-      <c r="O4" s="210"/>
-      <c r="P4" s="210"/>
-      <c r="Q4" s="210"/>
-      <c r="R4" s="212"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="189"/>
     </row>
     <row r="5" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="228" t="s">
+      <c r="B5" s="223"/>
+      <c r="C5" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="213" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="214"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="214" t="s">
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="214"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="213" t="s">
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="190" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="214"/>
-      <c r="N5" s="214"/>
-      <c r="O5" s="214"/>
-      <c r="P5" s="214"/>
-      <c r="Q5" s="214"/>
-      <c r="R5" s="215"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="192"/>
       <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="187">
-        <f>COUNTIF(E21:HM21,"P")</f>
+      <c r="A6" s="210">
+        <f>COUNTIF(E22:HM22,"P")</f>
         <v>2</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="227">
-        <f>COUNTIF(E21:HO21,"F")</f>
+      <c r="B6" s="211"/>
+      <c r="C6" s="204">
+        <f>COUNTIF(E22:HO22,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="216">
+      <c r="D6" s="194"/>
+      <c r="E6" s="193">
         <f>SUM(L6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="217"/>
-      <c r="G6" s="217"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="148">
-        <f>COUNTIF(E20:HM20,"N")</f>
+        <f>COUNTIF(E21:HM21,"N")</f>
         <v>1</v>
       </c>
       <c r="J6" s="148">
-        <f>COUNTIF(E20:HM20,"A")</f>
+        <f>COUNTIF(E21:HM21,"A")</f>
         <v>1</v>
       </c>
       <c r="K6" s="148">
-        <f>COUNTIF(E20:HO20,"B")</f>
+        <f>COUNTIF(E21:HO21,"B")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="216">
+      <c r="L6" s="193">
         <f>COUNTA(E8:R8)</f>
         <v>2</v>
       </c>
-      <c r="M6" s="217"/>
-      <c r="N6" s="217"/>
-      <c r="O6" s="217"/>
-      <c r="P6" s="217"/>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="218"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="149"/>
     </row>
     <row r="7" spans="1:20" ht="11.25" thickBot="1"/>
@@ -10114,7 +10145,9 @@
       </c>
       <c r="C9" s="117"/>
       <c r="D9" s="118"/>
-      <c r="E9" s="125"/>
+      <c r="E9" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="F9" s="106"/>
       <c r="G9" s="106"/>
       <c r="H9" s="125"/>
@@ -10137,7 +10170,9 @@
       <c r="C10" s="117"/>
       <c r="D10" s="118"/>
       <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
+      <c r="F10" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="G10" s="125"/>
       <c r="H10" s="125"/>
       <c r="I10" s="125"/>
@@ -10178,7 +10213,9 @@
     <row r="12" spans="1:20" ht="13.5" customHeight="1">
       <c r="A12" s="112"/>
       <c r="B12" s="116"/>
-      <c r="C12" s="117"/>
+      <c r="C12" s="117" t="s">
+        <v>156</v>
+      </c>
       <c r="D12" s="118">
         <v>1</v>
       </c>
@@ -10199,7 +10236,7 @@
       <c r="Q12" s="150"/>
       <c r="R12" s="124"/>
     </row>
-    <row r="13" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+    <row r="13" spans="1:20" ht="13.5" customHeight="1">
       <c r="A13" s="112"/>
       <c r="B13" s="116"/>
       <c r="C13" s="117"/>
@@ -10223,43 +10260,47 @@
       <c r="Q13" s="150"/>
       <c r="R13" s="124"/>
     </row>
-    <row r="14" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A14" s="114" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="80" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="125"/>
+    <row r="14" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A14" s="112"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="117" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="118" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="F14" s="125" t="s">
         <v>71</v>
       </c>
       <c r="G14" s="125"/>
       <c r="H14" s="125"/>
       <c r="I14" s="125"/>
-      <c r="J14" s="125"/>
-      <c r="K14" s="125"/>
-      <c r="L14" s="125"/>
-      <c r="M14" s="152"/>
-      <c r="N14" s="152"/>
-      <c r="O14" s="152"/>
-      <c r="P14" s="152"/>
-      <c r="Q14" s="152"/>
-      <c r="R14" s="125"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="150"/>
+      <c r="N14" s="150"/>
+      <c r="O14" s="150"/>
+      <c r="P14" s="150"/>
+      <c r="Q14" s="150"/>
+      <c r="R14" s="124"/>
     </row>
     <row r="15" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A15" s="113"/>
+      <c r="A15" s="114" t="s">
+        <v>54</v>
+      </c>
       <c r="B15" s="80" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C15" s="81"/>
       <c r="D15" s="82"/>
-      <c r="E15" s="125" t="s">
+      <c r="E15" s="125"/>
+      <c r="F15" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="125"/>
       <c r="G15" s="125"/>
       <c r="H15" s="125"/>
       <c r="I15" s="125"/>
@@ -10275,8 +10316,8 @@
     </row>
     <row r="16" spans="1:20" ht="13.5" customHeight="1">
       <c r="A16" s="113"/>
-      <c r="B16" s="83" t="s">
-        <v>124</v>
+      <c r="B16" s="80" t="s">
+        <v>132</v>
       </c>
       <c r="C16" s="81"/>
       <c r="D16" s="82"/>
@@ -10299,36 +10340,40 @@
     </row>
     <row r="17" spans="1:18" ht="13.5" customHeight="1">
       <c r="A17" s="113"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="D17" s="85">
-        <v>1</v>
-      </c>
-      <c r="E17" s="106" t="s">
+      <c r="B17" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="81"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="151"/>
-      <c r="N17" s="151"/>
-      <c r="O17" s="151"/>
-      <c r="P17" s="151"/>
-      <c r="Q17" s="151"/>
-      <c r="R17" s="106"/>
+      <c r="F17" s="125"/>
+      <c r="G17" s="125"/>
+      <c r="H17" s="125"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="125"/>
+      <c r="K17" s="125"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="152"/>
+      <c r="N17" s="152"/>
+      <c r="O17" s="152"/>
+      <c r="P17" s="152"/>
+      <c r="Q17" s="152"/>
+      <c r="R17" s="125"/>
     </row>
     <row r="18" spans="1:18" ht="13.5" customHeight="1">
       <c r="A18" s="113"/>
       <c r="B18" s="83"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="106"/>
+      <c r="C18" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="85">
+        <v>1</v>
+      </c>
+      <c r="E18" s="106" t="s">
+        <v>71</v>
+      </c>
       <c r="F18" s="106"/>
       <c r="G18" s="106"/>
       <c r="H18" s="106"/>
@@ -10336,137 +10381,149 @@
       <c r="J18" s="106"/>
       <c r="K18" s="106"/>
       <c r="L18" s="106"/>
-      <c r="M18" s="154"/>
-      <c r="N18" s="154"/>
-      <c r="O18" s="154"/>
-      <c r="P18" s="154"/>
-      <c r="Q18" s="154"/>
-      <c r="R18" s="155"/>
-    </row>
-    <row r="19" spans="1:18" ht="13.5" customHeight="1" thickBot="1">
+      <c r="M18" s="151"/>
+      <c r="N18" s="151"/>
+      <c r="O18" s="151"/>
+      <c r="P18" s="151"/>
+      <c r="Q18" s="151"/>
+      <c r="R18" s="106"/>
+    </row>
+    <row r="19" spans="1:18" ht="13.5" customHeight="1">
       <c r="A19" s="113"/>
       <c r="B19" s="83"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="152"/>
-      <c r="G19" s="152"/>
-      <c r="H19" s="152"/>
-      <c r="I19" s="152"/>
-      <c r="J19" s="152"/>
-      <c r="K19" s="152"/>
-      <c r="L19" s="152"/>
-      <c r="M19" s="152"/>
-      <c r="N19" s="152"/>
-      <c r="O19" s="152"/>
-      <c r="P19" s="152"/>
-      <c r="Q19" s="152"/>
-      <c r="R19" s="152"/>
-    </row>
-    <row r="20" spans="1:18" ht="13.5" customHeight="1" thickTop="1">
-      <c r="A20" s="114" t="s">
+      <c r="C19" s="117" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="118" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="106" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="154"/>
+      <c r="N19" s="154"/>
+      <c r="O19" s="154"/>
+      <c r="P19" s="154"/>
+      <c r="Q19" s="154"/>
+      <c r="R19" s="155"/>
+    </row>
+    <row r="20" spans="1:18" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A20" s="113"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="152"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="152"/>
+      <c r="J20" s="152"/>
+      <c r="K20" s="152"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="152"/>
+      <c r="N20" s="152"/>
+      <c r="O20" s="152"/>
+      <c r="P20" s="152"/>
+      <c r="Q20" s="152"/>
+      <c r="R20" s="152"/>
+    </row>
+    <row r="21" spans="1:18" ht="13.5" customHeight="1" thickTop="1">
+      <c r="A21" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="219" t="s">
+      <c r="B21" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="220"/>
-      <c r="D20" s="221"/>
-      <c r="E20" s="158" t="s">
+      <c r="C21" s="197"/>
+      <c r="D21" s="198"/>
+      <c r="E21" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="158" t="s">
+      <c r="F21" s="158" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="158"/>
-      <c r="K20" s="158"/>
-      <c r="L20" s="158"/>
-      <c r="M20" s="158"/>
-      <c r="N20" s="158"/>
-      <c r="O20" s="158"/>
-      <c r="P20" s="158"/>
-      <c r="Q20" s="158"/>
-      <c r="R20" s="158"/>
-    </row>
-    <row r="21" spans="1:18" ht="13.5" customHeight="1">
-      <c r="A21" s="113"/>
-      <c r="B21" s="222" t="s">
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158"/>
+      <c r="J21" s="158"/>
+      <c r="K21" s="158"/>
+      <c r="L21" s="158"/>
+      <c r="M21" s="158"/>
+      <c r="N21" s="158"/>
+      <c r="O21" s="158"/>
+      <c r="P21" s="158"/>
+      <c r="Q21" s="158"/>
+      <c r="R21" s="158"/>
+    </row>
+    <row r="22" spans="1:18" ht="13.5" customHeight="1">
+      <c r="A22" s="113"/>
+      <c r="B22" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="223"/>
-      <c r="D21" s="224"/>
-      <c r="E21" s="106" t="s">
+      <c r="C22" s="200"/>
+      <c r="D22" s="201"/>
+      <c r="E22" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="106" t="s">
+      <c r="F22" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="106"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="106"/>
-      <c r="N21" s="106"/>
-      <c r="O21" s="106"/>
-      <c r="P21" s="106"/>
-      <c r="Q21" s="106"/>
-      <c r="R21" s="106"/>
-    </row>
-    <row r="22" spans="1:18" ht="64.5" customHeight="1">
-      <c r="A22" s="113"/>
-      <c r="B22" s="207" t="s">
+      <c r="G22" s="106"/>
+      <c r="H22" s="106"/>
+      <c r="I22" s="106"/>
+      <c r="J22" s="106"/>
+      <c r="K22" s="106"/>
+      <c r="L22" s="106"/>
+      <c r="M22" s="106"/>
+      <c r="N22" s="106"/>
+      <c r="O22" s="106"/>
+      <c r="P22" s="106"/>
+      <c r="Q22" s="106"/>
+      <c r="R22" s="106"/>
+    </row>
+    <row r="23" spans="1:18" ht="64.5" customHeight="1">
+      <c r="A23" s="113"/>
+      <c r="B23" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="208"/>
-      <c r="D22" s="209"/>
-      <c r="E22" s="86">
+      <c r="C23" s="185"/>
+      <c r="D23" s="186"/>
+      <c r="E23" s="86">
         <v>42335</v>
       </c>
-      <c r="F22" s="86">
+      <c r="F23" s="86">
         <v>42335</v>
       </c>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="86"/>
-      <c r="L22" s="86"/>
-      <c r="M22" s="86"/>
-      <c r="N22" s="86"/>
-      <c r="O22" s="86"/>
-      <c r="P22" s="86"/>
-      <c r="Q22" s="86"/>
-      <c r="R22" s="86"/>
-    </row>
-    <row r="23" spans="1:18" ht="13.5" customHeight="1">
-      <c r="A23" s="111"/>
-    </row>
-    <row r="40" ht="24" customHeight="1"/>
-    <row r="41" ht="39" customHeight="1"/>
-    <row r="53" ht="57" customHeight="1"/>
-    <row r="54" ht="10.5"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="86"/>
+      <c r="P23" s="86"/>
+      <c r="Q23" s="86"/>
+      <c r="R23" s="86"/>
+    </row>
+    <row r="24" spans="1:18" ht="13.5" customHeight="1">
+      <c r="A24" s="111"/>
+    </row>
+    <row r="41" ht="24" customHeight="1"/>
+    <row r="42" ht="39" customHeight="1"/>
+    <row r="54" ht="57" customHeight="1"/>
     <row r="55" ht="10.5"/>
+    <row r="56" ht="10.5"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="L6:R6"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:R5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -10475,15 +10532,29 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:R3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10 I9 E9:G10 E11:R19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10 I9 E9:G10 E11:R20">
       <formula1>"O, "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21:R21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22:R22">
       <formula1>"P,F, "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20:R20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21:R21">
       <formula1>"N,A,B, "</formula1>
     </dataValidation>
   </dataValidations>
@@ -10500,7 +10571,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -10520,136 +10591,136 @@
       <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="185" t="s">
+      <c r="B2" s="207"/>
+      <c r="C2" s="208" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="186"/>
-      <c r="E2" s="201" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="224" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="191" t="str">
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="214" t="str">
         <f>C2</f>
         <v>DeleteSlide</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="193"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
+      <c r="O2" s="215"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="216"/>
       <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="197" t="str">
+      <c r="B3" s="213"/>
+      <c r="C3" s="220" t="str">
         <f>Cover!F4</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="D3" s="198"/>
-      <c r="E3" s="204" t="s">
+      <c r="D3" s="221"/>
+      <c r="E3" s="227" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="194" t="str">
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="229"/>
+      <c r="I3" s="217" t="str">
         <f>C3</f>
         <v>ManhLNSE02619</v>
       </c>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="196"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218"/>
+      <c r="R3" s="219"/>
     </row>
     <row r="4" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="210"/>
-      <c r="K4" s="210"/>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
-      <c r="N4" s="210"/>
-      <c r="O4" s="210"/>
-      <c r="P4" s="210"/>
-      <c r="Q4" s="210"/>
-      <c r="R4" s="212"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="189"/>
     </row>
     <row r="5" spans="1:20" ht="13.5" customHeight="1">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="222" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="228" t="s">
+      <c r="B5" s="223"/>
+      <c r="C5" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="214"/>
-      <c r="E5" s="213" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="214"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="225"/>
-      <c r="I5" s="214" t="s">
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="191" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="214"/>
-      <c r="K5" s="214"/>
-      <c r="L5" s="213" t="s">
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="190" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="214"/>
-      <c r="N5" s="214"/>
-      <c r="O5" s="214"/>
-      <c r="P5" s="214"/>
-      <c r="Q5" s="214"/>
-      <c r="R5" s="215"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="192"/>
       <c r="T5" s="78"/>
     </row>
     <row r="6" spans="1:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A6" s="187">
+      <c r="A6" s="210">
         <f>COUNTIF(E20:HM20,"P")</f>
         <v>2</v>
       </c>
-      <c r="B6" s="188"/>
-      <c r="C6" s="227">
+      <c r="B6" s="211"/>
+      <c r="C6" s="204">
         <f>COUNTIF(E20:HO20,"F")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="217"/>
-      <c r="E6" s="216">
+      <c r="D6" s="194"/>
+      <c r="E6" s="193">
         <f>SUM(L6,- A6,- C6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="217"/>
-      <c r="G6" s="217"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="148">
         <f>COUNTIF(E19:HM19,"N")</f>
         <v>1</v>
@@ -10662,16 +10733,16 @@
         <f>COUNTIF(E19:HO19,"B")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="216">
+      <c r="L6" s="193">
         <f>COUNTA(E8:R8)</f>
         <v>2</v>
       </c>
-      <c r="M6" s="217"/>
-      <c r="N6" s="217"/>
-      <c r="O6" s="217"/>
-      <c r="P6" s="217"/>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="218"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="149"/>
     </row>
     <row r="7" spans="1:20" ht="11.25" thickBot="1"/>
@@ -10709,7 +10780,9 @@
       </c>
       <c r="C9" s="117"/>
       <c r="D9" s="118"/>
-      <c r="E9" s="125"/>
+      <c r="E9" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="F9" s="106"/>
       <c r="G9" s="106"/>
       <c r="H9" s="125"/>
@@ -10732,7 +10805,9 @@
       <c r="C10" s="117"/>
       <c r="D10" s="118"/>
       <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
+      <c r="F10" s="125" t="s">
+        <v>71</v>
+      </c>
       <c r="G10" s="125"/>
       <c r="H10" s="125"/>
       <c r="I10" s="125"/>
@@ -10936,11 +11011,11 @@
       <c r="A19" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="219" t="s">
+      <c r="B19" s="196" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="220"/>
-      <c r="D19" s="221"/>
+      <c r="C19" s="197"/>
+      <c r="D19" s="198"/>
       <c r="E19" s="158" t="s">
         <v>37</v>
       </c>
@@ -10962,11 +11037,11 @@
     </row>
     <row r="20" spans="1:18" ht="13.5" customHeight="1">
       <c r="A20" s="113"/>
-      <c r="B20" s="222" t="s">
+      <c r="B20" s="199" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="223"/>
-      <c r="D20" s="224"/>
+      <c r="C20" s="200"/>
+      <c r="D20" s="201"/>
       <c r="E20" s="106" t="s">
         <v>41</v>
       </c>
@@ -10988,11 +11063,11 @@
     </row>
     <row r="21" spans="1:18" ht="64.5" customHeight="1">
       <c r="A21" s="113"/>
-      <c r="B21" s="207" t="s">
+      <c r="B21" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="208"/>
-      <c r="D21" s="209"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="186"/>
       <c r="E21" s="86">
         <v>42335</v>
       </c>
@@ -11022,20 +11097,6 @@
     <row r="54" ht="10.5"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="L6:R6"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:R5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -11044,6 +11105,20 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:R3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19:R19">

</xml_diff>